<commit_message>
defined some more apiservice calls for bonuses, started defining the extras that perks give
</commit_message>
<xml_diff>
--- a/docs/benefittables/tables.xlsx
+++ b/docs/benefittables/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7335" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7335" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -850,7 +850,7 @@
   <dimension ref="B1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,13 +1157,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="8" max="8" width="47.28515625" customWidth="1"/>
   </cols>
@@ -1405,12 +1405,12 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1648,12 +1648,12 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="93" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1891,12 +1891,12 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="86.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2191,12 +2191,12 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="102.7109375" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2415,12 +2415,12 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" customWidth="1"/>
     <col min="4" max="4" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2695,13 +2695,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
made skill purchasing load correctly, and changed api to be put/delete. defined framework feature edges
</commit_message>
<xml_diff>
--- a/docs/benefittables/tables.xlsx
+++ b/docs/benefittables/tables.xlsx
@@ -9,26 +9,29 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7335" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7335" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="underworld" sheetId="8" r:id="rId2"/>
-    <sheet name="training" sheetId="7" r:id="rId3"/>
-    <sheet name="psionics" sheetId="5" r:id="rId4"/>
-    <sheet name="ranged weapons" sheetId="6" r:id="rId5"/>
-    <sheet name="magic+mysticism" sheetId="4" r:id="rId6"/>
-    <sheet name="items+gadgets" sheetId="2" r:id="rId7"/>
-    <sheet name="xp+wisdom" sheetId="3" r:id="rId8"/>
+    <sheet name="providededge" sheetId="9" r:id="rId2"/>
+    <sheet name="edgechoice" sheetId="10" r:id="rId3"/>
+    <sheet name="bonuses" sheetId="11" r:id="rId4"/>
+    <sheet name="underworld" sheetId="8" r:id="rId5"/>
+    <sheet name="training" sheetId="7" r:id="rId6"/>
+    <sheet name="psionics" sheetId="5" r:id="rId7"/>
+    <sheet name="ranged weapons" sheetId="6" r:id="rId8"/>
+    <sheet name="magic+mysticism" sheetId="4" r:id="rId9"/>
+    <sheet name="items+gadgets" sheetId="2" r:id="rId10"/>
+    <sheet name="xp+wisdom" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'magic+mysticism'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">psionics!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ranged weapons'!$A$1:$C$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'magic+mysticism'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">psionics!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'ranged weapons'!$A$1:$C$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$C$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">training!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">underworld!$A$1:$C$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'xp+wisdom'!$A$1:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">training!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">underworld!$A$1:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'xp+wisdom'!$A$1:$C$13</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -40,20 +43,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="202">
   <si>
     <t>Made of a wood unknown to most of the world, your character’s elegant staff is a powerful weapon and tool for magic work. The staff has 10 PPE (which regenerate at the same rate as the caster), grants a +1 to all spellcasting rolls for AB: Magic and AB: Miracles, and contains two spells (powers) of the player’s choice, which can come from any list. Finally, it’s a combat-worthy staff (Str+d6, Reach 1, Parry +1, twohanded) that even does Mega Damage if 2 PPE is channeled through it that round.</t>
   </si>
   <si>
-    <t>Things get ugly out in the world, and the Ley Line Walker Medium Armor is a good insurance policy for dealing with a lot of those things. Cyber-Knights should re-roll on this result. 4 Going covert is much easier with a Shadow Cloak on. 5 – 6 Great for both damaging and slowing down enemies, an Iceblast Shotgun is an arcane favorite.</t>
-  </si>
-  <si>
     <t>When it’s time to negotiate with strange visitors just arrived through a new Rift, your character’s Communications Band is a vital asset. This upgraded item also enhances the user’s vocal output, granting him a +2 Charisma whenever he is speaking or otherwise using his voice.</t>
   </si>
   <si>
-    <t>Your hero is in good shape with a TW Shard Pistol at her side. 11 For up-close and personal encounters, a Flaming Sword is a good thing to have. It’s also great for barbecues.</t>
-  </si>
-  <si>
     <t>A cunning pair of goggles that speaks of a fashion that never goes out of style, your character’s Magic Optic System is a favorite accessory.</t>
   </si>
   <si>
@@ -520,6 +517,138 @@
   </si>
   <si>
     <t>SQL</t>
+  </si>
+  <si>
+    <t>Things get ugly out in the world, and the Ley Line Walker Medium Armor is a good insurance policy for dealing with a lot of those things. Cyber-Knights should re-roll on this result.</t>
+  </si>
+  <si>
+    <t>Your hero is in good shape with a TW Shard Pistol at her side.</t>
+  </si>
+  <si>
+    <t>perk type</t>
+  </si>
+  <si>
+    <t>parry_bonus</t>
+  </si>
+  <si>
+    <t>isp_bonus</t>
+  </si>
+  <si>
+    <t>ppe_bonus</t>
+  </si>
+  <si>
+    <t>num_languages_bonus</t>
+  </si>
+  <si>
+    <t>max_times_chosen</t>
+  </si>
+  <si>
+    <t>MCGUYVER</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>provided</t>
+  </si>
+  <si>
+    <t>backup</t>
+  </si>
+  <si>
+    <t>edge_category</t>
+  </si>
+  <si>
+    <t>I_KNOW_A_GUY</t>
+  </si>
+  <si>
+    <t>DIRTY_FIGHTER</t>
+  </si>
+  <si>
+    <t>TRICKY_FIGHTER</t>
+  </si>
+  <si>
+    <t>THIEF</t>
+  </si>
+  <si>
+    <t>SCROUNGER</t>
+  </si>
+  <si>
+    <t>JACK_OF_ALL_TRADES</t>
+  </si>
+  <si>
+    <t>ASSASSIN</t>
+  </si>
+  <si>
+    <t>BRAWLER</t>
+  </si>
+  <si>
+    <t>MARTIAL_ARTIST</t>
+  </si>
+  <si>
+    <t>IMPROVED_MARTIAL_ARTIST</t>
+  </si>
+  <si>
+    <t>PROFESSIONAL</t>
+  </si>
+  <si>
+    <t>WOODSMAN</t>
+  </si>
+  <si>
+    <t>COMBAT</t>
+  </si>
+  <si>
+    <t>must_obey_edge_reqs</t>
+  </si>
+  <si>
+    <t>ACE</t>
+  </si>
+  <si>
+    <t>COMBAT_ACE</t>
+  </si>
+  <si>
+    <t>WILD_CARD</t>
+  </si>
+  <si>
+    <t>SOUL_DRAIN</t>
+  </si>
+  <si>
+    <t>RAPID_RECHARGE</t>
+  </si>
+  <si>
+    <t>IMPROVED_RAPID_RECHARGE</t>
+  </si>
+  <si>
+    <t>MENTALIST</t>
+  </si>
+  <si>
+    <t>MARKSMAN</t>
+  </si>
+  <si>
+    <t>ELAN</t>
+  </si>
+  <si>
+    <t>STRONG_WILLED</t>
+  </si>
+  <si>
+    <t>COMMON_BOND</t>
+  </si>
+  <si>
+    <t>DANGER_SENSE</t>
+  </si>
+  <si>
+    <t>QUICK</t>
+  </si>
+  <si>
+    <t>LEVEL_HEADED</t>
+  </si>
+  <si>
+    <t>BACKGROUND</t>
+  </si>
+  <si>
+    <t>LUCK</t>
+  </si>
+  <si>
+    <t>GREAT_LUCK</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1282,1199 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="65.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Made of a wood unknown to most of the world, your character’s elegant staff is a powerful weapon and tool for magic work. The staff has 10 PPE (which regenerate at the same rate as the caster), grants a +1 to all spellcasting rolls for AB: Magic and AB: Miracles, and contains two spells (powers) of the player’s choice, which can come from any list. Finally, it’s a combat-worthy staff (Str+d6, Reach 1, Parry +1, twohanded) that even does Mega Damage if 2 PPE is channeled through it that round.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_1');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_1_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E14" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Things get ugly out in the world, and the Ley Line Walker Medium Armor is a good insurance policy for dealing with a lot of those things. Cyber-Knights should re-roll on this result.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_2');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_2_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Going covert is much easier with a Shadow Cloak on. ', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_3');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_3_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Great for both damaging and slowing down enemies, an Iceblast Shotgun is an arcane favorite.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_4');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_4_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('When it’s time to negotiate with strange visitors just arrived through a new Rift, your character’s Communications Band is a vital asset. This upgraded item also enhances the user’s vocal output, granting him a +2 Charisma whenever he is speaking or otherwise using his voice.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_5');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_5_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Your hero is in good shape with a TW Shard Pistol at her side.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_6');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_6_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('For up-close and personal encounters, a Flaming Sword is a good thing to have. It’s also great for barbecues.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_7');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_7_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('A cunning pair of goggles that speaks of a fashion that never goes out of style, your character’s Magic Optic System is a favorite accessory.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_8');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_8_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('The TK Revolver is a favorite among Techno-Wizards and those who don’t like keeping up with ammunition.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_9');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_9_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Your hero has a rare and coveted suit of TW Combat Mage Armor, which may or may not place him on a few bounty lists in both the Coalition and the Federation of Magic. Alternately, if he’s a Cyber-Knight, he gains a suit of TW Cyber-Knight Heavy Armor.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_10');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_10_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('One of the nastier weapons created by Techno-Wizards, the Draining Blade is just the thing for evening the odds against a superior physical combatant.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_11');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_11_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Whether your character’s a Techno-Wizard or just wants to travel like one, the Wingboard is a great choice for him.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_12');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_12_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('You may choose any one of the previous results.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_13');
+SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_13_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="94.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Your hero knows how to make the most of second chances. He has Elan.', 'EXPERIENCE_WISDOM_1');
+SET @EXPERIENCE_WISDOM_1_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E13" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Your character doesn’t take kindly to threats, and no one messes with her head. She is Strong Willed.', 'EXPERIENCE_WISDOM_2');
+SET @EXPERIENCE_WISDOM_2_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('With a nose for opportunities, horse-trading, and five-fingered discounts, your hero is the go-to person for getting what’s needed in a crunch. He has the Scrounger Edge and Connections (Black Market).', 'EXPERIENCE_WISDOM_3');
+SET @EXPERIENCE_WISDOM_3_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Some folks come to understand that lone wolves don’t make it in a world as dangerous as this one. Your hero has Common Bond.', 'EXPERIENCE_WISDOM_4');
+SET @EXPERIENCE_WISDOM_4_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('She always gets a strange tingling in the back of her neck when things are about to go all pear-shaped. She’s seen enough trouble to know when it’s coming. Your character has the Danger Sense Edge.', 'EXPERIENCE_WISDOM_5');
+SET @EXPERIENCE_WISDOM_5_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('A split second often means the difference between alive and a smear on the landscape. Your character has the Quick Edge. If he already has that Edge, he gains the Level Headed Edge instead.', 'EXPERIENCE_WISDOM_6');
+SET @EXPERIENCE_WISDOM_6_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Some experiences take a person back to the beginning, reconnecting her to her foundations. Select one Background Edge, regardless of requirements, so long as it makes sense and the GM agrees with it.', 'EXPERIENCE_WISDOM_7');
+SET @EXPERIENCE_WISDOM_7_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('He’s traveled far and wide, and he knows a lot about the world that could come in handy. Your character gains a +2 on any Common Knowledge rolls related to geography and understanding the people and places of North America. He also gains a +2 on Survival and Streetwise checks in North America.', 'EXPERIENCE_WISDOM_8');
+SET @EXPERIENCE_WISDOM_8_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('There are times when no amount of skill, talent, or training is enough. Fortunately for your character, she has a bit of Luck (as in the Edge) on her side. Take Great Luck instead if she already has Luck.', 'EXPERIENCE_WISDOM_9');
+SET @EXPERIENCE_WISDOM_9_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('Life on the road, in the wilderness, and wandering the streets of the cities that remain gave your character special insight and some key experience with a particular calling. You may give her one Professional Edge, ignoring requirements, subject to the GM’s approval and it making at least some kind of sense.', 'EXPERIENCE_WISDOM_10');
+SET @EXPERIENCE_WISDOM_10_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('There are moments when everything comes together and an opportunity presents itself. Your hero knows how to make the most of just such a moment; choose one Wild Card Edge, regardless of requirements.', 'EXPERIENCE_WISDOM_11');
+SET @EXPERIENCE_WISDOM_11_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk` (description, type) VALUES ('You may choose any one of the previous results.', 'EXPERIENCE_WISDOM_12');
+SET @EXPERIENCE_WISDOM_12_ID = LAST_INSERT_ID();</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C13"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D2:D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = '"&amp;A2&amp;"'), (SELECT id FROM edge WHERE edge_type='"&amp;B2&amp;"'),  (SELECT id FROM edge WHERE edge_type='"&amp;C2&amp;"'));"</f>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_1'), (SELECT id FROM edge WHERE edge_type='MCGUYVER'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D26" si="0">"INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = '"&amp;A3&amp;"'), (SELECT id FROM edge WHERE edge_type='"&amp;B3&amp;"'),  (SELECT id FROM edge WHERE edge_type='"&amp;C3&amp;"'));"</f>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_3'), (SELECT id FROM edge WHERE edge_type='I_KNOW_A_GUY'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_4'), (SELECT id FROM edge WHERE edge_type='DIRTY_FIGHTER'),  (SELECT id FROM edge WHERE edge_type='TRICKY_FIGHTER'));</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_6'), (SELECT id FROM edge WHERE edge_type='THIEF'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_8'), (SELECT id FROM edge WHERE edge_type='SCROUNGER'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_9'), (SELECT id FROM edge WHERE edge_type='JACK_OF_ALL_TRADES'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'UNDERWORLD_BLACK_OPS_10'), (SELECT id FROM edge WHERE edge_type='ASSASSIN'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_2'), (SELECT id FROM edge WHERE edge_type='MARTIAL_ARTIST'),  (SELECT id FROM edge WHERE edge_type='IMPROVED_MARTIAL_ARTIST'));</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_2'), (SELECT id FROM edge WHERE edge_type='BRAWLER'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_4'), (SELECT id FROM edge WHERE edge_type='WOODSMAN'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_7'), (SELECT id FROM edge WHERE edge_type='DIRTY_FIGHTER'),  (SELECT id FROM edge WHERE edge_type='TRICKY_FIGHTER'));</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_9'), (SELECT id FROM edge WHERE edge_type='ACE'),  (SELECT id FROM edge WHERE edge_type='COMBAT_ACE'));</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'PSIONICS_1'), (SELECT id FROM edge WHERE edge_type='SOUL_DRAIN'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'PSIONICS_2'), (SELECT id FROM edge WHERE edge_type='RAPID_RECHARGE'),  (SELECT id FROM edge WHERE edge_type='IMPROVED_RAPID_RECHARGE'));</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'PSIONICS_8'), (SELECT id FROM edge WHERE edge_type='MENTALIST'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'MAGIC_MYSTICISM_1'), (SELECT id FROM edge WHERE edge_type='SOUL_DRAIN'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'MAGIC_MYSTICISM_2'), (SELECT id FROM edge WHERE edge_type='MARKSMAN'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'MAGIC_MYSTICISM_5'), (SELECT id FROM edge WHERE edge_type='RAPID_RECHARGE'),  (SELECT id FROM edge WHERE edge_type='IMPROVED_RAPID_RECHARGE'));</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_1'), (SELECT id FROM edge WHERE edge_type='ELAN'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_2'), (SELECT id FROM edge WHERE edge_type='STRONG_WILLED'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_3'), (SELECT id FROM edge WHERE edge_type='SCROUNGER'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_4'), (SELECT id FROM edge WHERE edge_type='COMMON_BOND'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_5'), (SELECT id FROM edge WHERE edge_type='DANGER_SENSE'),  (SELECT id FROM edge WHERE edge_type=''));</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_6'), (SELECT id FROM edge WHERE edge_type='QUICK'),  (SELECT id FROM edge WHERE edge_type='LEVEL_HEADED'));</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_provided_edge` (perk, provided_edge, backup_edge) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_9'), (SELECT id FROM edge WHERE edge_type='LUCK'),  (SELECT id FROM edge WHERE edge_type='GREAT_LUCK'));</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = '"&amp;A2&amp;"'), '"&amp;B2&amp;"');"</f>
+        <v>INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_3'), 'PROFESSIONAL');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D7" si="0">"INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = '"&amp;A3&amp;"'), '"&amp;B3&amp;"');"</f>
+        <v>INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_8'), 'COMBAT');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = 'TRAINING_10'), 'WILD_CARD');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_7'), 'BACKGROUND');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_10'), 'PROFESSIONAL');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `perk_edge_choice` (perk, edge_category) VALUES ((SELECT id FROM perk WHERE type = 'EXPERIENCE_WISDOM_11'), 'WILD_CARD');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"UPDATE `perk` SET parry_bonus = "&amp;B2&amp;", isp_bonus="&amp;C2&amp;", ppe_bonus="&amp;D2&amp;", num_languages_bonus="&amp;E2&amp;", max_times_chosen="&amp;F2&amp;" WHERE type = '"&amp;A2&amp;"';"</f>
+        <v>UPDATE `perk` SET parry_bonus = NULL, isp_bonus=NULL, ppe_bonus=NULL, num_languages_bonus=2, max_times_chosen=NULL WHERE type = 'UNDERWORLD_BLACK_OPS_7';</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G7" si="0">"UPDATE `perk` SET parry_bonus = "&amp;B3&amp;", isp_bonus="&amp;C3&amp;", ppe_bonus="&amp;D3&amp;", num_languages_bonus="&amp;E3&amp;", max_times_chosen="&amp;F3&amp;" WHERE type = '"&amp;A3&amp;"';"</f>
+        <v>UPDATE `perk` SET parry_bonus = 1, isp_bonus=NULL, ppe_bonus=NULL, num_languages_bonus=NULL, max_times_chosen=NULL WHERE type = 'TRAINING_7';</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE `perk` SET parry_bonus = NULL, isp_bonus=10, ppe_bonus=NULL, num_languages_bonus=NULL, max_times_chosen=NULL WHERE type = 'PSIONICS_3';</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE `perk` SET parry_bonus = NULL, isp_bonus=NULL, ppe_bonus=NULL, num_languages_bonus=NULL, max_times_chosen=2 WHERE type = 'RANGED_WEAPONS_3';</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE `perk` SET parry_bonus = NULL, isp_bonus=NULL, ppe_bonus=NULL, num_languages_bonus=NULL, max_times_chosen=3 WHERE type = 'RANGED_WEAPONS_5';</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE `perk` SET parry_bonus = NULL, isp_bonus=NULL, ppe_bonus=5, num_languages_bonus=NULL, max_times_chosen=NULL WHERE type = 'MAGIC_MYSTICISM_3';</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -1170,16 +2491,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1190,10 +2511,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1210,10 +2531,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E12" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1230,10 +2551,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1249,10 +2570,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1268,10 +2589,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1287,10 +2608,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1306,10 +2627,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -1325,10 +2646,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -1344,10 +2665,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -1363,10 +2684,10 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -1382,10 +2703,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -1400,7 +2721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -1416,16 +2737,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,10 +2757,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1455,10 +2776,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E12" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1474,10 +2795,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1493,10 +2814,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1512,10 +2833,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1531,10 +2852,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1550,10 +2871,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -1569,10 +2890,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -1588,10 +2909,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -1607,10 +2928,10 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -1626,10 +2947,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -1643,7 +2964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -1659,16 +2980,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1679,10 +3000,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1698,10 +3019,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E12" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1717,10 +3038,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1736,10 +3057,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1755,10 +3076,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1774,10 +3095,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1793,10 +3114,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -1812,10 +3133,10 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -1831,10 +3152,10 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -1850,10 +3171,10 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -1869,10 +3190,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -1886,7 +3207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -1902,16 +3223,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1922,10 +3243,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1941,10 +3262,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E15" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -1960,10 +3281,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1979,10 +3300,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1998,10 +3319,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -2017,10 +3338,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -2036,10 +3357,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -2055,10 +3376,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -2074,10 +3395,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -2093,10 +3414,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -2112,10 +3433,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -2131,10 +3452,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -2150,10 +3471,10 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -2169,10 +3490,10 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -2186,7 +3507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2202,16 +3523,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2222,10 +3543,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -2241,10 +3562,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E11" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
@@ -2260,10 +3581,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -2279,10 +3600,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -2298,10 +3619,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -2317,10 +3638,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -2336,10 +3657,10 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -2355,10 +3676,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -2374,10 +3695,10 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -2393,10 +3714,10 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -2408,548 +3729,4 @@
   <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="65.85546875" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Made of a wood unknown to most of the world, your character’s elegant staff is a powerful weapon and tool for magic work. The staff has 10 PPE (which regenerate at the same rate as the caster), grants a +1 to all spellcasting rolls for AB: Magic and AB: Miracles, and contains two spells (powers) of the player’s choice, which can come from any list. Finally, it’s a combat-worthy staff (Str+d6, Reach 1, Parry +1, twohanded) that even does Mega Damage if 2 PPE is channeled through it that round.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_1');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_1_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E14" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Things get ugly out in the world, and the Ley Line Walker Medium Armor is a good insurance policy for dealing with a lot of those things. Cyber-Knights should re-roll on this result. 4 Going covert is much easier with a Shadow Cloak on. 5 – 6 Great for both damaging and slowing down enemies, an Iceblast Shotgun is an arcane favorite.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_2');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_2_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Going covert is much easier with a Shadow Cloak on. ', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_3');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_3_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Great for both damaging and slowing down enemies, an Iceblast Shotgun is an arcane favorite.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_4');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_4_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('When it’s time to negotiate with strange visitors just arrived through a new Rift, your character’s Communications Band is a vital asset. This upgraded item also enhances the user’s vocal output, granting him a +2 Charisma whenever he is speaking or otherwise using his voice.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_5');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_5_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Your hero is in good shape with a TW Shard Pistol at her side. 11 For up-close and personal encounters, a Flaming Sword is a good thing to have. It’s also great for barbecues.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_6');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_6_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('For up-close and personal encounters, a Flaming Sword is a good thing to have. It’s also great for barbecues.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_7');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_7_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('A cunning pair of goggles that speaks of a fashion that never goes out of style, your character’s Magic Optic System is a favorite accessory.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_8');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_8_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('The TK Revolver is a favorite among Techno-Wizards and those who don’t like keeping up with ammunition.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_9');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_9_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Your hero has a rare and coveted suit of TW Combat Mage Armor, which may or may not place him on a few bounty lists in both the Coalition and the Federation of Magic. Alternately, if he’s a Cyber-Knight, he gains a suit of TW Cyber-Knight Heavy Armor.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_10');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_10_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('One of the nastier weapons created by Techno-Wizards, the Draining Blade is just the thing for evening the odds against a superior physical combatant.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_11');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_11_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Whether your character’s a Techno-Wizard or just wants to travel like one, the Wingboard is a great choice for him.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_12');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_12_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('You may choose any one of the previous results.', 'ENCHANTED_ITEMS_MYSTIC_GADGETS_13');
-SET @ENCHANTED_ITEMS_MYSTIC_GADGETS_13_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="94.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"INSERT INTO `perk` (description, type) VALUES ('"&amp;C2&amp;"', '"&amp;D2&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D2&amp;"_ID = LAST_INSERT_ID();"</f>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Your hero knows how to make the most of second chances. He has Elan.', 'EXPERIENCE_WISDOM_1');
-SET @EXPERIENCE_WISDOM_1_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E13" si="0">"INSERT INTO `perk` (description, type) VALUES ('"&amp;C3&amp;"', '"&amp;D3&amp;"');"&amp;CHAR(10)&amp;"SET @"&amp;D3&amp;"_ID = LAST_INSERT_ID();"</f>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Your character doesn’t take kindly to threats, and no one messes with her head. She is Strong Willed.', 'EXPERIENCE_WISDOM_2');
-SET @EXPERIENCE_WISDOM_2_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('With a nose for opportunities, horse-trading, and five-fingered discounts, your hero is the go-to person for getting what’s needed in a crunch. He has the Scrounger Edge and Connections (Black Market).', 'EXPERIENCE_WISDOM_3');
-SET @EXPERIENCE_WISDOM_3_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Some folks come to understand that lone wolves don’t make it in a world as dangerous as this one. Your hero has Common Bond.', 'EXPERIENCE_WISDOM_4');
-SET @EXPERIENCE_WISDOM_4_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('She always gets a strange tingling in the back of her neck when things are about to go all pear-shaped. She’s seen enough trouble to know when it’s coming. Your character has the Danger Sense Edge.', 'EXPERIENCE_WISDOM_5');
-SET @EXPERIENCE_WISDOM_5_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('A split second often means the difference between alive and a smear on the landscape. Your character has the Quick Edge. If he already has that Edge, he gains the Level Headed Edge instead.', 'EXPERIENCE_WISDOM_6');
-SET @EXPERIENCE_WISDOM_6_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Some experiences take a person back to the beginning, reconnecting her to her foundations. Select one Background Edge, regardless of requirements, so long as it makes sense and the GM agrees with it.', 'EXPERIENCE_WISDOM_7');
-SET @EXPERIENCE_WISDOM_7_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('He’s traveled far and wide, and he knows a lot about the world that could come in handy. Your character gains a +2 on any Common Knowledge rolls related to geography and understanding the people and places of North America. He also gains a +2 on Survival and Streetwise checks in North America.', 'EXPERIENCE_WISDOM_8');
-SET @EXPERIENCE_WISDOM_8_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('There are times when no amount of skill, talent, or training is enough. Fortunately for your character, she has a bit of Luck (as in the Edge) on her side. Take Great Luck instead if she already has Luck.', 'EXPERIENCE_WISDOM_9');
-SET @EXPERIENCE_WISDOM_9_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('Life on the road, in the wilderness, and wandering the streets of the cities that remain gave your character special insight and some key experience with a particular calling. You may give her one Professional Edge, ignoring requirements, subject to the GM’s approval and it making at least some kind of sense.', 'EXPERIENCE_WISDOM_10');
-SET @EXPERIENCE_WISDOM_10_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('There are moments when everything comes together and an opportunity presents itself. Your hero knows how to make the most of just such a moment; choose one Wild Card Edge, regardless of requirements.', 'EXPERIENCE_WISDOM_11');
-SET @EXPERIENCE_WISDOM_11_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO `perk` (description, type) VALUES ('You may choose any one of the previous results.', 'EXPERIENCE_WISDOM_12');
-SET @EXPERIENCE_WISDOM_12_ID = LAST_INSERT_ID();</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C13"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>